<commit_message>
docs:added graphs for analysis
</commit_message>
<xml_diff>
--- a/graph/clean_data1.xlsx
+++ b/graph/clean_data1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="28">
   <si>
     <t>input case</t>
   </si>
@@ -67,7 +67,10 @@
     <t>Merge</t>
   </si>
   <si>
-    <t>BIQuick</t>
+    <t>Built-in Quick</t>
+  </si>
+  <si>
+    <t>Own Quick</t>
   </si>
   <si>
     <t>OwnQuick</t>
@@ -85,7 +88,7 @@
     <t>Gen Heap</t>
   </si>
   <si>
-    <t>Gen Quick</t>
+    <t>Gen Own Quick</t>
   </si>
   <si>
     <t>Gen Merge</t>
@@ -98,7 +101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -110,19 +113,32 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -145,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -154,6 +170,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -372,7 +391,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="7" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -865,16 +884,16 @@
       <c r="B22" s="2">
         <v>10000.0</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>0.041</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>0.039</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>0.039</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>0.039666</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -888,16 +907,16 @@
       <c r="B23" s="2">
         <v>20000.0</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>0.162</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>0.154</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>0.153</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>0.156333</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -911,16 +930,16 @@
       <c r="B24" s="2">
         <v>40000.0</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>0.614</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>0.614</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>0.629</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>0.619</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -934,16 +953,16 @@
       <c r="B25" s="2">
         <v>80000.0</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>2.473</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>2.401</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>2.421</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>0.248833333</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -3177,7 +3196,7 @@
       <c r="F122" s="2">
         <v>0.0</v>
       </c>
-      <c r="G122" s="2" t="s">
+      <c r="G122" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3200,7 +3219,7 @@
       <c r="F123" s="2">
         <v>0.0</v>
       </c>
-      <c r="G123" s="2" t="s">
+      <c r="G123" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3223,7 +3242,7 @@
       <c r="F124" s="2">
         <v>0.001333333333</v>
       </c>
-      <c r="G124" s="2" t="s">
+      <c r="G124" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3246,7 +3265,7 @@
       <c r="F125" s="2">
         <v>0.003</v>
       </c>
-      <c r="G125" s="2" t="s">
+      <c r="G125" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3269,7 +3288,7 @@
       <c r="F126" s="2">
         <v>3.333333333E-4</v>
       </c>
-      <c r="G126" s="2" t="s">
+      <c r="G126" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3292,7 +3311,7 @@
       <c r="F127" s="2">
         <v>0.002</v>
       </c>
-      <c r="G127" s="2" t="s">
+      <c r="G127" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3315,7 +3334,7 @@
       <c r="F128" s="2">
         <v>0.004</v>
       </c>
-      <c r="G128" s="2" t="s">
+      <c r="G128" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3338,7 +3357,7 @@
       <c r="F129" s="2">
         <v>0.007333333333</v>
       </c>
-      <c r="G129" s="2" t="s">
+      <c r="G129" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3361,7 +3380,7 @@
       <c r="F130" s="2">
         <v>6.666666667E-4</v>
       </c>
-      <c r="G130" s="2" t="s">
+      <c r="G130" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3384,7 +3403,7 @@
       <c r="F131" s="2">
         <v>0.001666666667</v>
       </c>
-      <c r="G131" s="2" t="s">
+      <c r="G131" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3407,7 +3426,7 @@
       <c r="F132" s="2">
         <v>0.003</v>
       </c>
-      <c r="G132" s="2" t="s">
+      <c r="G132" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3430,7 +3449,7 @@
       <c r="F133" s="2">
         <v>0.006666666667</v>
       </c>
-      <c r="G133" s="2" t="s">
+      <c r="G133" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3453,7 +3472,7 @@
       <c r="F134" s="2">
         <v>0.001</v>
       </c>
-      <c r="G134" s="2" t="s">
+      <c r="G134" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3476,7 +3495,7 @@
       <c r="F135" s="2">
         <v>0.001666666667</v>
       </c>
-      <c r="G135" s="2" t="s">
+      <c r="G135" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3499,7 +3518,7 @@
       <c r="F136" s="2">
         <v>0.003333333333</v>
       </c>
-      <c r="G136" s="2" t="s">
+      <c r="G136" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3522,7 +3541,7 @@
       <c r="F137" s="2">
         <v>0.007</v>
       </c>
-      <c r="G137" s="2" t="s">
+      <c r="G137" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3545,7 +3564,7 @@
       <c r="F138" s="2">
         <v>0.0</v>
       </c>
-      <c r="G138" s="2" t="s">
+      <c r="G138" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3568,7 +3587,7 @@
       <c r="F139" s="2">
         <v>3.333333333E-4</v>
       </c>
-      <c r="G139" s="2" t="s">
+      <c r="G139" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3591,7 +3610,7 @@
       <c r="F140" s="2">
         <v>0.001666666667</v>
       </c>
-      <c r="G140" s="2" t="s">
+      <c r="G140" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3614,7 +3633,7 @@
       <c r="F141" s="2">
         <v>0.003</v>
       </c>
-      <c r="G141" s="2" t="s">
+      <c r="G141" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3637,7 +3656,7 @@
       <c r="F142" s="2">
         <v>0.0</v>
       </c>
-      <c r="G142" s="2" t="s">
+      <c r="G142" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3661,7 +3680,7 @@
         <v>6.666666667E-4</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="144" ht="15.75" customHeight="1">
@@ -3683,7 +3702,7 @@
       <c r="F144" s="2">
         <v>0.001333333333</v>
       </c>
-      <c r="G144" s="2" t="s">
+      <c r="G144" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3706,7 +3725,7 @@
       <c r="F145" s="2">
         <v>0.003333333333</v>
       </c>
-      <c r="G145" s="2" t="s">
+      <c r="G145" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3729,7 +3748,7 @@
       <c r="F146" s="2">
         <v>0.0</v>
       </c>
-      <c r="G146" s="2" t="s">
+      <c r="G146" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3752,7 +3771,7 @@
       <c r="F147" s="2">
         <v>0.001</v>
       </c>
-      <c r="G147" s="2" t="s">
+      <c r="G147" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3775,7 +3794,7 @@
       <c r="F148" s="2">
         <v>0.003</v>
       </c>
-      <c r="G148" s="2" t="s">
+      <c r="G148" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3798,7 +3817,7 @@
       <c r="F149" s="2">
         <v>0.006666666667</v>
       </c>
-      <c r="G149" s="2" t="s">
+      <c r="G149" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3821,7 +3840,7 @@
       <c r="F150" s="2">
         <v>3.333333333E-4</v>
       </c>
-      <c r="G150" s="2" t="s">
+      <c r="G150" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3844,7 +3863,7 @@
       <c r="F151" s="2">
         <v>0.001333333333</v>
       </c>
-      <c r="G151" s="2" t="s">
+      <c r="G151" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3867,7 +3886,7 @@
       <c r="F152" s="2">
         <v>0.003</v>
       </c>
-      <c r="G152" s="2" t="s">
+      <c r="G152" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3890,7 +3909,7 @@
       <c r="F153" s="2">
         <v>0.007</v>
       </c>
-      <c r="G153" s="2" t="s">
+      <c r="G153" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3913,7 +3932,7 @@
       <c r="F154" s="2">
         <v>6.666666667E-4</v>
       </c>
-      <c r="G154" s="2" t="s">
+      <c r="G154" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3936,7 +3955,7 @@
       <c r="F155" s="2">
         <v>0.001666666667</v>
       </c>
-      <c r="G155" s="2" t="s">
+      <c r="G155" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3959,7 +3978,7 @@
       <c r="F156" s="2">
         <v>0.003333333333</v>
       </c>
-      <c r="G156" s="2" t="s">
+      <c r="G156" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3982,7 +4001,7 @@
       <c r="F157" s="2">
         <v>0.008333333333</v>
       </c>
-      <c r="G157" s="2" t="s">
+      <c r="G157" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4005,7 +4024,7 @@
       <c r="F158" s="2">
         <v>3.333333333E-4</v>
       </c>
-      <c r="G158" s="2" t="s">
+      <c r="G158" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4028,7 +4047,7 @@
       <c r="F159" s="2">
         <v>0.001</v>
       </c>
-      <c r="G159" s="2" t="s">
+      <c r="G159" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4051,7 +4070,7 @@
       <c r="F160" s="2">
         <v>0.002</v>
       </c>
-      <c r="G160" s="2" t="s">
+      <c r="G160" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4074,7 +4093,7 @@
       <c r="F161" s="2">
         <v>0.004</v>
       </c>
-      <c r="G161" s="2" t="s">
+      <c r="G161" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4098,7 +4117,7 @@
         <v>0.0</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="163" ht="15.75" customHeight="1">
@@ -4121,7 +4140,7 @@
         <v>0.0</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="164" ht="15.75" customHeight="1">
@@ -4144,7 +4163,7 @@
         <v>0.0</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="165" ht="15.75" customHeight="1">
@@ -4167,7 +4186,7 @@
         <v>6.666666667E-4</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="166" ht="15.75" customHeight="1">
@@ -4190,7 +4209,7 @@
         <v>0.8366666667</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="167" ht="15.75" customHeight="1">
@@ -4213,7 +4232,7 @@
         <v>3.356</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="168" ht="15.75" customHeight="1">
@@ -4236,7 +4255,7 @@
         <v>13.957</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="169" ht="15.75" customHeight="1">
@@ -4259,7 +4278,7 @@
         <v>61.41233333</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="170" ht="15.75" customHeight="1">
@@ -4282,7 +4301,7 @@
         <v>0.8183333333</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="171" ht="15.75" customHeight="1">
@@ -4305,7 +4324,7 @@
         <v>3.249666667</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="172" ht="15.75" customHeight="1">
@@ -4328,7 +4347,7 @@
         <v>14.032</v>
       </c>
       <c r="G172" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="173" ht="15.75" customHeight="1">
@@ -4351,7 +4370,7 @@
         <v>64.35866667</v>
       </c>
       <c r="G173" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="174" ht="15.75" customHeight="1">
@@ -4374,7 +4393,7 @@
         <v>0.8073333333</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="175" ht="15.75" customHeight="1">
@@ -4397,7 +4416,7 @@
         <v>3.382666667</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="176" ht="15.75" customHeight="1">
@@ -4420,7 +4439,7 @@
         <v>13.84066667</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="177" ht="15.75" customHeight="1">
@@ -4443,7 +4462,7 @@
         <v>61.83666667</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="178" ht="15.75" customHeight="1">
@@ -4466,7 +4485,7 @@
         <v>1.743</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="179" ht="15.75" customHeight="1">
@@ -4489,7 +4508,7 @@
         <v>6.917333333</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="180" ht="15.75" customHeight="1">
@@ -4512,7 +4531,7 @@
         <v>28.14133333</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="181" ht="15.75" customHeight="1">
@@ -4535,7 +4554,7 @@
         <v>94.567</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="182" ht="15.75" customHeight="1">
@@ -4545,20 +4564,20 @@
       <c r="B182" s="2">
         <v>10000.0</v>
       </c>
-      <c r="C182" s="3">
+      <c r="C182" s="2">
         <v>0.065</v>
       </c>
-      <c r="D182" s="3">
+      <c r="D182" s="2">
         <v>0.071</v>
       </c>
-      <c r="E182" s="3">
+      <c r="E182" s="2">
         <v>0.07</v>
       </c>
-      <c r="F182" s="3">
+      <c r="F182" s="2">
         <v>0.068666</v>
       </c>
       <c r="G182" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="183" ht="15.75" customHeight="1">
@@ -4568,20 +4587,20 @@
       <c r="B183" s="2">
         <v>20000.0</v>
       </c>
-      <c r="C183" s="3">
+      <c r="C183" s="2">
         <v>0.261</v>
       </c>
-      <c r="D183" s="3">
+      <c r="D183" s="2">
         <v>0.259</v>
       </c>
-      <c r="E183" s="3">
+      <c r="E183" s="2">
         <v>0.259</v>
       </c>
-      <c r="F183" s="3">
+      <c r="F183" s="2">
         <v>0.25966666</v>
       </c>
       <c r="G183" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="184" ht="15.75" customHeight="1">
@@ -4591,20 +4610,20 @@
       <c r="B184" s="2">
         <v>40000.0</v>
       </c>
-      <c r="C184" s="3">
+      <c r="C184" s="2">
         <v>1.068</v>
       </c>
-      <c r="D184" s="3">
+      <c r="D184" s="2">
         <v>1.048</v>
       </c>
-      <c r="E184" s="3">
+      <c r="E184" s="2">
         <v>1.08</v>
       </c>
-      <c r="F184" s="3">
+      <c r="F184" s="2">
         <v>1.06533333</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="185" ht="15.75" customHeight="1">
@@ -4614,20 +4633,20 @@
       <c r="B185" s="2">
         <v>80000.0</v>
       </c>
-      <c r="C185" s="3">
+      <c r="C185" s="2">
         <v>4.152</v>
       </c>
-      <c r="D185" s="3">
+      <c r="D185" s="2">
         <v>4.171</v>
       </c>
-      <c r="E185" s="3">
+      <c r="E185" s="2">
         <v>4.128</v>
       </c>
-      <c r="F185" s="3">
+      <c r="F185" s="2">
         <v>4.1503333333</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="186" ht="15.75" customHeight="1">
@@ -4650,7 +4669,7 @@
         <v>0.9073333333</v>
       </c>
       <c r="G186" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="187" ht="15.75" customHeight="1">
@@ -4673,7 +4692,7 @@
         <v>3.670333333</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="188" ht="15.75" customHeight="1">
@@ -4696,7 +4715,7 @@
         <v>15.995</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="189" ht="15.75" customHeight="1">
@@ -4719,7 +4738,7 @@
         <v>62.15966667</v>
       </c>
       <c r="G189" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="190" ht="15.75" customHeight="1">
@@ -4742,7 +4761,7 @@
         <v>0.905</v>
       </c>
       <c r="G190" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="191" ht="15.75" customHeight="1">
@@ -4765,7 +4784,7 @@
         <v>3.693666667</v>
       </c>
       <c r="G191" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="192" ht="15.75" customHeight="1">
@@ -4788,7 +4807,7 @@
         <v>15.08766667</v>
       </c>
       <c r="G192" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="193" ht="15.75" customHeight="1">
@@ -4811,7 +4830,7 @@
         <v>61.83333333</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="194" ht="15.75" customHeight="1">
@@ -4834,7 +4853,7 @@
         <v>0.932</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="195" ht="15.75" customHeight="1">
@@ -4857,7 +4876,7 @@
         <v>3.683333333</v>
       </c>
       <c r="G195" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="196" ht="15.75" customHeight="1">
@@ -4880,7 +4899,7 @@
         <v>14.907</v>
       </c>
       <c r="G196" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="197" ht="15.75" customHeight="1">
@@ -4903,7 +4922,7 @@
         <v>61.64933333</v>
       </c>
       <c r="G197" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="198" ht="15.75" customHeight="1">
@@ -4926,7 +4945,7 @@
         <v>1.501333333</v>
       </c>
       <c r="G198" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="199" ht="15.75" customHeight="1">
@@ -4949,7 +4968,7 @@
         <v>6.104333333</v>
       </c>
       <c r="G199" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="200" ht="15.75" customHeight="1">
@@ -4972,7 +4991,7 @@
         <v>23.87433333</v>
       </c>
       <c r="G200" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="201" ht="15.75" customHeight="1">
@@ -4995,7 +5014,7 @@
         <v>95.15</v>
       </c>
       <c r="G201" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="202" ht="15.75" customHeight="1">
@@ -5018,7 +5037,7 @@
         <v>0.07366666667</v>
       </c>
       <c r="G202" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="203" ht="15.75" customHeight="1">
@@ -5041,7 +5060,7 @@
         <v>0.29</v>
       </c>
       <c r="G203" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="204" ht="15.75" customHeight="1">
@@ -5064,7 +5083,7 @@
         <v>1.128666667</v>
       </c>
       <c r="G204" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="205" ht="15.75" customHeight="1">
@@ -5087,7 +5106,7 @@
         <v>4.509666667</v>
       </c>
       <c r="G205" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="206" ht="15.75" customHeight="1">
@@ -5110,7 +5129,7 @@
         <v>0.074</v>
       </c>
       <c r="G206" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="207" ht="15.75" customHeight="1">
@@ -5133,7 +5152,7 @@
         <v>0.291</v>
       </c>
       <c r="G207" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="208" ht="15.75" customHeight="1">
@@ -5156,7 +5175,7 @@
         <v>1.150333333</v>
       </c>
       <c r="G208" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="209" ht="15.75" customHeight="1">
@@ -5179,7 +5198,7 @@
         <v>4.377333333</v>
       </c>
       <c r="G209" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="210" ht="15.75" customHeight="1">
@@ -5202,7 +5221,7 @@
         <v>0.07366666667</v>
       </c>
       <c r="G210" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="211" ht="15.75" customHeight="1">
@@ -5225,7 +5244,7 @@
         <v>0.286</v>
       </c>
       <c r="G211" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="212" ht="15.75" customHeight="1">
@@ -5248,7 +5267,7 @@
         <v>1.138666667</v>
       </c>
       <c r="G212" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="213" ht="15.75" customHeight="1">
@@ -5271,7 +5290,7 @@
         <v>4.376666667</v>
       </c>
       <c r="G213" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="214" ht="15.75" customHeight="1">
@@ -5294,7 +5313,7 @@
         <v>0.074</v>
       </c>
       <c r="G214" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="215" ht="15.75" customHeight="1">
@@ -5317,7 +5336,7 @@
         <v>0.287</v>
       </c>
       <c r="G215" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="216" ht="15.75" customHeight="1">
@@ -5340,7 +5359,7 @@
         <v>1.124666667</v>
       </c>
       <c r="G216" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="217" ht="15.75" customHeight="1">
@@ -5363,7 +5382,7 @@
         <v>4.371333333</v>
       </c>
       <c r="G217" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="218" ht="15.75" customHeight="1">
@@ -5386,7 +5405,7 @@
         <v>0.07</v>
       </c>
       <c r="G218" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="219" ht="15.75" customHeight="1">
@@ -5409,7 +5428,7 @@
         <v>0.274</v>
       </c>
       <c r="G219" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="220" ht="15.75" customHeight="1">
@@ -5432,7 +5451,7 @@
         <v>1.076</v>
       </c>
       <c r="G220" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="221" ht="15.75" customHeight="1">
@@ -5455,7 +5474,7 @@
         <v>4.217333333</v>
       </c>
       <c r="G221" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="222" ht="15.75" customHeight="1">
@@ -5478,7 +5497,7 @@
         <v>0.005333333333</v>
       </c>
       <c r="G222" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="223" ht="15.75" customHeight="1">
@@ -5501,7 +5520,7 @@
         <v>0.01033333333</v>
       </c>
       <c r="G223" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="224" ht="15.75" customHeight="1">
@@ -5524,7 +5543,7 @@
         <v>0.022</v>
       </c>
       <c r="G224" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="225" ht="15.75" customHeight="1">
@@ -5547,7 +5566,7 @@
         <v>0.04733333333</v>
       </c>
       <c r="G225" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="226" ht="15.75" customHeight="1">
@@ -5570,7 +5589,7 @@
         <v>0.005</v>
       </c>
       <c r="G226" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="227" ht="15.75" customHeight="1">
@@ -5593,7 +5612,7 @@
         <v>0.01133333333</v>
       </c>
       <c r="G227" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="228" ht="15.75" customHeight="1">
@@ -5616,7 +5635,7 @@
         <v>0.024</v>
       </c>
       <c r="G228" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="229" ht="15.75" customHeight="1">
@@ -5639,7 +5658,7 @@
         <v>0.048</v>
       </c>
       <c r="G229" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="230" ht="15.75" customHeight="1">
@@ -5662,7 +5681,7 @@
         <v>0.005</v>
       </c>
       <c r="G230" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="231" ht="15.75" customHeight="1">
@@ -5685,7 +5704,7 @@
         <v>0.01166666667</v>
       </c>
       <c r="G231" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="232" ht="15.75" customHeight="1">
@@ -5708,7 +5727,7 @@
         <v>0.02366666667</v>
       </c>
       <c r="G232" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="233" ht="15.75" customHeight="1">
@@ -5731,7 +5750,7 @@
         <v>0.048</v>
       </c>
       <c r="G233" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="234" ht="15.75" customHeight="1">
@@ -5754,7 +5773,7 @@
         <v>0.005</v>
       </c>
       <c r="G234" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="235" ht="15.75" customHeight="1">
@@ -5777,7 +5796,7 @@
         <v>0.01133333333</v>
       </c>
       <c r="G235" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="236" ht="15.75" customHeight="1">
@@ -5800,7 +5819,7 @@
         <v>0.02333333333</v>
       </c>
       <c r="G236" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="237" ht="15.75" customHeight="1">
@@ -5823,7 +5842,7 @@
         <v>0.04833333333</v>
       </c>
       <c r="G237" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="238" ht="15.75" customHeight="1">
@@ -5846,7 +5865,7 @@
         <v>0.004333333333</v>
       </c>
       <c r="G238" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="239" ht="15.75" customHeight="1">
@@ -5869,7 +5888,7 @@
         <v>0.01</v>
       </c>
       <c r="G239" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="240" ht="15.75" customHeight="1">
@@ -5892,7 +5911,7 @@
         <v>0.02066666667</v>
       </c>
       <c r="G240" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="241" ht="15.75" customHeight="1">
@@ -5915,7 +5934,7 @@
         <v>0.04266666667</v>
       </c>
       <c r="G241" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="242" ht="15.75" customHeight="1">
@@ -5937,8 +5956,8 @@
       <c r="F242" s="2">
         <v>0.003</v>
       </c>
-      <c r="G242" s="2" t="s">
-        <v>24</v>
+      <c r="G242" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="243" ht="15.75" customHeight="1">
@@ -5960,8 +5979,8 @@
       <c r="F243" s="2">
         <v>0.006666666667</v>
       </c>
-      <c r="G243" s="2" t="s">
-        <v>24</v>
+      <c r="G243" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="244" ht="15.75" customHeight="1">
@@ -5983,8 +6002,8 @@
       <c r="F244" s="2">
         <v>0.01566666667</v>
       </c>
-      <c r="G244" s="2" t="s">
-        <v>24</v>
+      <c r="G244" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="245" ht="15.75" customHeight="1">
@@ -6006,8 +6025,8 @@
       <c r="F245" s="2">
         <v>0.03033333333</v>
       </c>
-      <c r="G245" s="2" t="s">
-        <v>24</v>
+      <c r="G245" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="246" ht="15.75" customHeight="1">
@@ -6029,8 +6048,8 @@
       <c r="F246" s="2">
         <v>0.003666666667</v>
       </c>
-      <c r="G246" s="2" t="s">
-        <v>24</v>
+      <c r="G246" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="247" ht="15.75" customHeight="1">
@@ -6052,8 +6071,8 @@
       <c r="F247" s="2">
         <v>0.007666666667</v>
       </c>
-      <c r="G247" s="2" t="s">
-        <v>24</v>
+      <c r="G247" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="248" ht="15.75" customHeight="1">
@@ -6075,8 +6094,8 @@
       <c r="F248" s="2">
         <v>0.01766666667</v>
       </c>
-      <c r="G248" s="2" t="s">
-        <v>24</v>
+      <c r="G248" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="249" ht="15.75" customHeight="1">
@@ -6098,8 +6117,8 @@
       <c r="F249" s="2">
         <v>0.034</v>
       </c>
-      <c r="G249" s="2" t="s">
-        <v>24</v>
+      <c r="G249" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="250" ht="15.75" customHeight="1">
@@ -6121,8 +6140,8 @@
       <c r="F250" s="2">
         <v>0.004</v>
       </c>
-      <c r="G250" s="2" t="s">
-        <v>24</v>
+      <c r="G250" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="251" ht="15.75" customHeight="1">
@@ -6144,8 +6163,8 @@
       <c r="F251" s="2">
         <v>0.007333333333</v>
       </c>
-      <c r="G251" s="2" t="s">
-        <v>24</v>
+      <c r="G251" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="252" ht="15.75" customHeight="1">
@@ -6167,8 +6186,8 @@
       <c r="F252" s="2">
         <v>0.017</v>
       </c>
-      <c r="G252" s="2" t="s">
-        <v>24</v>
+      <c r="G252" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="253" ht="15.75" customHeight="1">
@@ -6190,8 +6209,8 @@
       <c r="F253" s="2">
         <v>0.035</v>
       </c>
-      <c r="G253" s="2" t="s">
-        <v>24</v>
+      <c r="G253" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="254" ht="15.75" customHeight="1">
@@ -6213,8 +6232,8 @@
       <c r="F254" s="2">
         <v>0.003666666667</v>
       </c>
-      <c r="G254" s="2" t="s">
-        <v>24</v>
+      <c r="G254" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="255" ht="15.75" customHeight="1">
@@ -6236,8 +6255,8 @@
       <c r="F255" s="2">
         <v>0.007666666667</v>
       </c>
-      <c r="G255" s="2" t="s">
-        <v>24</v>
+      <c r="G255" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="256" ht="15.75" customHeight="1">
@@ -6259,8 +6278,8 @@
       <c r="F256" s="2">
         <v>0.01533333333</v>
       </c>
-      <c r="G256" s="2" t="s">
-        <v>24</v>
+      <c r="G256" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="257" ht="15.75" customHeight="1">
@@ -6282,8 +6301,8 @@
       <c r="F257" s="2">
         <v>0.03533333333</v>
       </c>
-      <c r="G257" s="2" t="s">
-        <v>24</v>
+      <c r="G257" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="258" ht="15.75" customHeight="1">
@@ -6305,8 +6324,8 @@
       <c r="F258" s="2">
         <v>0.003333333333</v>
       </c>
-      <c r="G258" s="2" t="s">
-        <v>24</v>
+      <c r="G258" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="259" ht="15.75" customHeight="1">
@@ -6328,8 +6347,8 @@
       <c r="F259" s="2">
         <v>0.006666666667</v>
       </c>
-      <c r="G259" s="2" t="s">
-        <v>24</v>
+      <c r="G259" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="260" ht="15.75" customHeight="1">
@@ -6351,8 +6370,8 @@
       <c r="F260" s="2">
         <v>0.014</v>
       </c>
-      <c r="G260" s="2" t="s">
-        <v>24</v>
+      <c r="G260" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="261" ht="15.75" customHeight="1">
@@ -6374,8 +6393,8 @@
       <c r="F261" s="2">
         <v>0.02866666667</v>
       </c>
-      <c r="G261" s="2" t="s">
-        <v>24</v>
+      <c r="G261" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="262" ht="15.75" customHeight="1">
@@ -6398,7 +6417,7 @@
         <v>6.666666667E-4</v>
       </c>
       <c r="G262" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="263" ht="15.75" customHeight="1">
@@ -6421,7 +6440,7 @@
         <v>0.001333333333</v>
       </c>
       <c r="G263" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="264" ht="15.75" customHeight="1">
@@ -6444,7 +6463,7 @@
         <v>0.002333333333</v>
       </c>
       <c r="G264" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="265" ht="15.75" customHeight="1">
@@ -6467,7 +6486,7 @@
         <v>0.006666666667</v>
       </c>
       <c r="G265" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="266" ht="15.75" customHeight="1">
@@ -6490,7 +6509,7 @@
         <v>0.001</v>
       </c>
       <c r="G266" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="267" ht="15.75" customHeight="1">
@@ -6513,7 +6532,7 @@
         <v>0.003</v>
       </c>
       <c r="G267" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="268" ht="15.75" customHeight="1">
@@ -6536,7 +6555,7 @@
         <v>0.006</v>
       </c>
       <c r="G268" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="269" ht="15.75" customHeight="1">
@@ -6559,7 +6578,7 @@
         <v>0.01233333333</v>
       </c>
       <c r="G269" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="270" ht="15.75" customHeight="1">
@@ -6582,7 +6601,7 @@
         <v>0.001666666667</v>
       </c>
       <c r="G270" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="271" ht="15.75" customHeight="1">
@@ -6605,7 +6624,7 @@
         <v>0.003</v>
       </c>
       <c r="G271" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="272" ht="15.75" customHeight="1">
@@ -6628,7 +6647,7 @@
         <v>0.006</v>
       </c>
       <c r="G272" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="273" ht="15.75" customHeight="1">
@@ -6651,7 +6670,7 @@
         <v>0.012</v>
       </c>
       <c r="G273" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="274" ht="15.75" customHeight="1">
@@ -6674,7 +6693,7 @@
         <v>0.001666666667</v>
       </c>
       <c r="G274" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="275" ht="15.75" customHeight="1">
@@ -6697,7 +6716,7 @@
         <v>0.003</v>
       </c>
       <c r="G275" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="276" ht="15.75" customHeight="1">
@@ -6720,7 +6739,7 @@
         <v>0.006</v>
       </c>
       <c r="G276" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="277" ht="15.75" customHeight="1">
@@ -6743,7 +6762,7 @@
         <v>0.01266666667</v>
       </c>
       <c r="G277" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="278" ht="15.75" customHeight="1">
@@ -6766,7 +6785,7 @@
         <v>3.333333333E-4</v>
       </c>
       <c r="G278" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="279" ht="15.75" customHeight="1">
@@ -6789,7 +6808,7 @@
         <v>0.002</v>
       </c>
       <c r="G279" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="280" ht="15.75" customHeight="1">
@@ -6812,7 +6831,7 @@
         <v>0.003333333333</v>
       </c>
       <c r="G280" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="281" ht="15.75" customHeight="1">
@@ -6835,7 +6854,7 @@
         <v>0.006666666667</v>
       </c>
       <c r="G281" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="282" ht="15.75" customHeight="1">
@@ -6858,7 +6877,7 @@
         <v>6.666666667E-4</v>
       </c>
       <c r="G282" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="283" ht="15.75" customHeight="1">
@@ -6881,7 +6900,7 @@
         <v>0.001</v>
       </c>
       <c r="G283" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="284" ht="15.75" customHeight="1">
@@ -6904,7 +6923,7 @@
         <v>0.001</v>
       </c>
       <c r="G284" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="285" ht="15.75" customHeight="1">
@@ -6927,7 +6946,7 @@
         <v>0.001</v>
       </c>
       <c r="G285" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="286" ht="15.75" customHeight="1">
@@ -6950,7 +6969,7 @@
         <v>0.006</v>
       </c>
       <c r="G286" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="287" ht="15.75" customHeight="1">
@@ -6973,7 +6992,7 @@
         <v>0.01333333333</v>
       </c>
       <c r="G287" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="288" ht="15.75" customHeight="1">
@@ -6996,7 +7015,7 @@
         <v>0.03466666667</v>
       </c>
       <c r="G288" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="289" ht="15.75" customHeight="1">
@@ -7019,7 +7038,7 @@
         <v>0.07966666667</v>
       </c>
       <c r="G289" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="290" ht="15.75" customHeight="1">
@@ -7042,7 +7061,7 @@
         <v>0.006</v>
       </c>
       <c r="G290" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="291" ht="15.75" customHeight="1">
@@ -7065,7 +7084,7 @@
         <v>0.01366666667</v>
       </c>
       <c r="G291" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="292" ht="15.75" customHeight="1">
@@ -7088,7 +7107,7 @@
         <v>0.03433333333</v>
       </c>
       <c r="G292" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="293" ht="15.75" customHeight="1">
@@ -7111,7 +7130,7 @@
         <v>0.07833333333</v>
       </c>
       <c r="G293" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="294" ht="15.75" customHeight="1">
@@ -7134,7 +7153,7 @@
         <v>0.005333333333</v>
       </c>
       <c r="G294" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="295" ht="15.75" customHeight="1">
@@ -7157,7 +7176,7 @@
         <v>0.013</v>
       </c>
       <c r="G295" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="296" ht="15.75" customHeight="1">
@@ -7180,7 +7199,7 @@
         <v>0.03266666667</v>
       </c>
       <c r="G296" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="297" ht="15.75" customHeight="1">
@@ -7203,7 +7222,7 @@
         <v>0.07733333333</v>
       </c>
       <c r="G297" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="298" ht="15.75" customHeight="1">
@@ -7226,7 +7245,7 @@
         <v>0.002333333333</v>
       </c>
       <c r="G298" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="299" ht="15.75" customHeight="1">
@@ -7249,7 +7268,7 @@
         <v>0.005333333333</v>
       </c>
       <c r="G299" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="300" ht="15.75" customHeight="1">
@@ -7272,7 +7291,7 @@
         <v>0.011</v>
       </c>
       <c r="G300" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="301" ht="15.75" customHeight="1">
@@ -7295,7 +7314,7 @@
         <v>0.023</v>
       </c>
       <c r="G301" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="302" ht="15.75" customHeight="1"/>

</xml_diff>